<commit_message>
express input corregidas hasta la 17
</commit_message>
<xml_diff>
--- a/TP1/Mediciones/glosario_magico.xlsx
+++ b/TP1/Mediciones/glosario_magico.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3847922B-6BB8-47B5-BBB7-814FFE125116}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A67821-2063-46A2-9A8C-5A0B77DB1436}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
   <si>
     <t>ARCHIVO</t>
   </si>
@@ -118,9 +124,6 @@
     <t>FAA + S&amp;H + FR - XA: Senoidal 500Hz 2Vpp - Duty 24%</t>
   </si>
   <si>
-    <t>FAA + LLAVE + FR - XA: Senoidal 500Hz 2Vpp - Duty 24%</t>
-  </si>
-  <si>
     <t>FAA + LLAVE + FR - XB: exp{-|t|} 10Hz 2V - Duty 20%</t>
   </si>
   <si>
@@ -145,9 +148,6 @@
     <t>FAA + S&amp;H + FR - XB: exp{-|t|} 10Hz 2V - Duty 10%</t>
   </si>
   <si>
-    <t>FAA + S&amp;H + FR - XA: Senoidal 1KHz 2Vpp - Duty 14%</t>
-  </si>
-  <si>
     <t>ITEM</t>
   </si>
   <si>
@@ -197,6 +197,42 @@
   </si>
   <si>
     <t>Señal sampleada</t>
+  </si>
+  <si>
+    <t>FAA + LLAVE + FR - XA: Senoidal 500Hz 6Vpp - Duty 24%</t>
+  </si>
+  <si>
+    <t>FAA + LLAVE - XB: exp{-|t|} 10Hz 2V - Duty 20%</t>
+  </si>
+  <si>
+    <t>FAA + S&amp;H - XB: exp{-|t|} 10Hz 2V - Duty 20%</t>
+  </si>
+  <si>
+    <t>FAA + S&amp;H - XA: Senoidal 500Hz 2Vpp - Duty 71%</t>
+  </si>
+  <si>
+    <t>FAA + LLAVE - XA: Senoidal 500Hz 2Vpp - Duty 88%</t>
+  </si>
+  <si>
+    <t>FAA + LLAVE - XB: exp{-|t|} 10Hz 2V - Duty 30%</t>
+  </si>
+  <si>
+    <t>FAA + S&amp;H - XA: Senoidal 1KHz 2Vpp - Duty 14%</t>
+  </si>
+  <si>
+    <t>FAA + S&amp;H - XA: Senoidal 500Hz 2Vpp - Duty 24%</t>
+  </si>
+  <si>
+    <t>FAA + LLAVE - XA: Senoidal 500Hz 2Vpp - Duty 24%</t>
+  </si>
+  <si>
+    <t>FAA + LLAVE - XA: 3/2 Seno 500Hz 2Vpp - Duty 44%</t>
+  </si>
+  <si>
+    <t>FAA + S&amp;H - XA: 3/2 Seno 500Hz 2Vpp - Duty 8%</t>
+  </si>
+  <si>
+    <t>FAA + LLA + S&amp;H - XC - Duty LLA 70% - Duty S&amp;H 10% - fs = 3KHz</t>
   </si>
 </sst>
 </file>
@@ -316,10 +352,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -605,18 +641,18 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="81.6640625" customWidth="1"/>
-    <col min="3" max="3" width="60.21875" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="81.7109375" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -627,24 +663,24 @@
         <v>29</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -654,228 +690,228 @@
       <c r="C3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="7"/>
-    </row>
-    <row r="16" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>30</v>
@@ -884,101 +920,101 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="D23" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="8"/>
-    </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="8"/>
-    </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="29" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
     </row>

</xml_diff>